<commit_message>
chore: change to report
</commit_message>
<xml_diff>
--- a/notebooks/1-preprocessing/ICA TO REMOVE.xlsx
+++ b/notebooks/1-preprocessing/ICA TO REMOVE.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Altair93/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/PhD/Projects/psd-path/notebooks/1-preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46ECE4D-1C0E-4E4E-B366-7F514FBB8AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBF60A6-3C9C-8E4F-BC72-032CDE73C52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="27980" windowHeight="17040" xr2:uid="{83A1080E-A454-6348-A3C2-92B7641F4505}"/>
+    <workbookView xWindow="3540" yWindow="740" windowWidth="27980" windowHeight="17040" xr2:uid="{83A1080E-A454-6348-A3C2-92B7641F4505}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>0 5 12 13 18 22 24</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>45 20 28</t>
   </si>
 </sst>
 </file>
@@ -235,14 +241,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -258,9 +263,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -298,7 +303,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -404,7 +409,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -546,7 +551,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -554,10 +559,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0C8EAD-5B96-664B-B05A-C8EB82CA9E16}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -566,15 +572,18 @@
     <col min="3" max="3" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>101</v>
       </c>
@@ -582,7 +591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4">
       <c r="A3">
         <f>A2+1</f>
         <v>102</v>
@@ -591,7 +600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4">
       <c r="A4">
         <f t="shared" ref="A4:A48" si="0">A3+1</f>
         <v>103</v>
@@ -600,7 +609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:4">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>104</v>
@@ -609,7 +618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:4">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>105</v>
@@ -618,7 +627,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:4">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>106</v>
@@ -627,7 +636,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:4">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>107</v>
@@ -636,7 +645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:4">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>108</v>
@@ -645,7 +654,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:4">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>109</v>
@@ -654,7 +663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:4">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>110</v>
@@ -663,7 +672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:4">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>111</v>
@@ -672,7 +681,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:4">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>112</v>
@@ -681,7 +690,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:4">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>113</v>
@@ -690,7 +699,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:4">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>114</v>
@@ -699,7 +708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:4">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>115</v>
@@ -708,7 +717,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:4">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>116</v>
@@ -717,7 +726,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>118</v>
       </c>
@@ -725,8 +734,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="3">
+    <row r="19" spans="1:4">
+      <c r="A19">
         <f t="shared" si="0"/>
         <v>119</v>
       </c>
@@ -734,7 +743,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:4">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>120</v>
@@ -743,7 +752,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>122</v>
       </c>
@@ -751,7 +760,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:4">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>123</v>
@@ -760,7 +769,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:4">
       <c r="A23">
         <f>A22+1</f>
         <v>124</v>
@@ -769,7 +778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:4">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>125</v>
@@ -778,7 +787,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:4">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>126</v>
@@ -787,7 +796,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:4">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>127</v>
@@ -796,7 +805,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:4">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>128</v>
@@ -805,7 +814,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:4">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>129</v>
@@ -814,15 +823,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>131</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="D29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>132</v>
@@ -831,7 +843,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>134</v>
       </c>
@@ -839,7 +851,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:4">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>135</v>

</xml_diff>